<commit_message>
Adjusted lab 4 rubric
Changed point distribution
</commit_message>
<xml_diff>
--- a/week 8 (Lab 4- Binomials and AIC)/Lab_4_rubric.xlsx
+++ b/week 8 (Lab 4- Binomials and AIC)/Lab_4_rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umainesystem-my.sharepoint.com/personal/liam_berigan_maine_edu/Documents/MaineAnalysis/WLE411/week 8 (Lab 4- Binomials and AIC)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38E0DA56-B0F5-4DE0-B18F-8ADF40B5D221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{38E0DA56-B0F5-4DE0-B18F-8ADF40B5D221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5A01B60-CA79-435D-AB5B-8F6BCC62E4EE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{E8E0656E-8A7A-479F-83C0-F394EAE37C22}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +514,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -566,7 +566,7 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>